<commit_message>
updated LoginPage to consume data from Excel sheet
</commit_message>
<xml_diff>
--- a/Ds-Algo/src/test/resources/TestData/registerUserName.xlsx
+++ b/Ds-Algo/src/test/resources/TestData/registerUserName.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sushm\eclipse-workspace\Ds-Algo\src\test\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seravi\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2716E60A-E73A-4DDF-84D9-4B01B7B94C40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C9DD6F3-39E6-40D6-971B-26BA78FF2F8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{D61A649E-4D94-4624-B804-336D99FF8C04}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{D61A649E-4D94-4624-B804-336D99FF8C04}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="validCredentials" sheetId="2" r:id="rId2"/>
+    <sheet name="invalidCredential" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
   <si>
     <t>username</t>
   </si>
@@ -80,6 +82,18 @@
   <si>
     <t>ds_algo_abs_ch_202</t>
   </si>
+  <si>
+    <t>abschallengers</t>
+  </si>
+  <si>
+    <t>numpyninja17</t>
+  </si>
+  <si>
+    <t>abschallengers123</t>
+  </si>
+  <si>
+    <t>numpyninja17123</t>
+  </si>
 </sst>
 </file>
 
@@ -89,7 +103,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -164,39 +178,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="0E2841"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E8E8E8"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="156082"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="E97132"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="196B24"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="0F9ED5"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="A02B93"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="4EA72E"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="467886"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="96607D"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -248,7 +262,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -359,6 +373,13 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -367,13 +388,6 @@
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -438,31 +452,11 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -472,18 +466,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1929D44-78B4-4671-9E60-A337D1DC7BCF}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.3125" customWidth="1"/>
-    <col min="3" max="3" width="23.47265625" customWidth="1"/>
+    <col min="1" max="1" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.26953125" customWidth="1"/>
+    <col min="3" max="3" width="23.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -494,7 +488,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -505,7 +499,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -516,7 +510,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -531,4 +525,90 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6CBD3A1-8FC8-4DFF-B1EE-932FD7F5D1A9}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5AC6ECB-E070-4576-BC94-2E2947905D24}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Array and linkedlist pages
</commit_message>
<xml_diff>
--- a/Ds-Algo/src/test/resources/TestData/registerUserName.xlsx
+++ b/Ds-Algo/src/test/resources/TestData/registerUserName.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omkku\Desktop\Bhuvana_Selenium\Ds-Algo\src\test\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seravi\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{963A7FC4-8A13-450D-BAC5-31BFCBF6F0E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EE7AB345-F614-48C1-A448-2438ADDBFA48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="24792" windowHeight="13320" activeTab="3" xr2:uid="{D61A649E-4D94-4624-B804-336D99FF8C04}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{D61A649E-4D94-4624-B804-336D99FF8C04}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="validCredentials" sheetId="2" r:id="rId2"/>
     <sheet name="invalidCredential" sheetId="3" r:id="rId3"/>
     <sheet name="Text_Try_Editor" sheetId="4" r:id="rId4"/>
+    <sheet name="practiceQuestions" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
   <si>
     <t>username</t>
   </si>
@@ -104,6 +105,47 @@
   </si>
   <si>
     <t>hello</t>
+  </si>
+  <si>
+    <t>invalidText</t>
+  </si>
+  <si>
+    <t>validText</t>
+  </si>
+  <si>
+    <t>Links</t>
+  </si>
+  <si>
+    <t>Search the array</t>
+  </si>
+  <si>
+    <t>Max Consecutive Ones</t>
+  </si>
+  <si>
+    <t>Find Numbers with Even Number</t>
+  </si>
+  <si>
+    <t>Squares of a Sorted Array</t>
+  </si>
+  <si>
+    <t>my_list = [1, 2, 3, 4, 5] # Element to check
+element = 3
+# Check if the element is in the list
+if element in my_list:
+    print("The element exists in the list.")
+else:
+    print("The element does not exist in the list.")</t>
+  </si>
+  <si>
+    <t>example = [22, 234, 2463]
+def is_even(value):
+    length = len(str(value))
+    return length % 2 == 0
+count = 0
+for i in example:
+    if is_even(i):
+        count += 1
+print(count)</t>
   </si>
 </sst>
 </file>
@@ -157,10 +199,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -628,8 +673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2362296-9E5A-4FF5-B377-523F7E4FFCF2}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -653,4 +698,79 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A89F3651-1282-425B-8D04-CB962D62DA53}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60.54296875" customWidth="1"/>
+    <col min="3" max="3" width="28.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="174" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="174" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="174" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding practice questions excel sheet
</commit_message>
<xml_diff>
--- a/Ds-Algo/src/test/resources/TestData/registerUserName.xlsx
+++ b/Ds-Algo/src/test/resources/TestData/registerUserName.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sushm\eclipse-workspace\Ds-Algo-Git\ABS-Challengers\Ds-Algo\src\test\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seravi\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4345BE77-A19A-48D4-9652-31A9D842B772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EE7AB345-F614-48C1-A448-2438ADDBFA48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{D61A649E-4D94-4624-B804-336D99FF8C04}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{D61A649E-4D94-4624-B804-336D99FF8C04}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="validCredentials" sheetId="2" r:id="rId2"/>
     <sheet name="invalidCredential" sheetId="3" r:id="rId3"/>
     <sheet name="Text_Try_Editor" sheetId="4" r:id="rId4"/>
+    <sheet name="practiceQuestions" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
   <si>
     <t>username</t>
   </si>
@@ -62,6 +63,26 @@
     </r>
   </si>
   <si>
+    <r>
+      <t>ds_algo_abs_ch_20</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <t>ds_algo_abs_ch_201</t>
+  </si>
+  <si>
+    <t>ds_algo_abs_ch_202</t>
+  </si>
+  <si>
     <t>abschallengers</t>
   </si>
   <si>
@@ -86,13 +107,45 @@
     <t>hello</t>
   </si>
   <si>
-    <t>ds_algo_abs_ch_210</t>
-  </si>
-  <si>
-    <t>ds_algo_abs_ch_211</t>
-  </si>
-  <si>
-    <t>ds_algo_abs_ch_212</t>
+    <t>invalidText</t>
+  </si>
+  <si>
+    <t>validText</t>
+  </si>
+  <si>
+    <t>Links</t>
+  </si>
+  <si>
+    <t>Search the array</t>
+  </si>
+  <si>
+    <t>Max Consecutive Ones</t>
+  </si>
+  <si>
+    <t>Find Numbers with Even Number</t>
+  </si>
+  <si>
+    <t>Squares of a Sorted Array</t>
+  </si>
+  <si>
+    <t>my_list = [1, 2, 3, 4, 5] # Element to check
+element = 3
+# Check if the element is in the list
+if element in my_list:
+    print("The element exists in the list.")
+else:
+    print("The element does not exist in the list.")</t>
+  </si>
+  <si>
+    <t>example = [22, 234, 2463]
+def is_even(value):
+    length = len(str(value))
+    return length % 2 == 0
+count = 0
+for i in example:
+    if is_even(i):
+        count += 1
+print(count)</t>
   </si>
 </sst>
 </file>
@@ -146,10 +199,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -168,9 +224,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -208,7 +264,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -314,7 +370,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -456,7 +512,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -466,18 +522,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1929D44-78B4-4671-9E60-A337D1DC7BCF}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.26171875" customWidth="1"/>
-    <col min="3" max="3" width="23.47265625" customWidth="1"/>
+    <col min="1" max="1" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.26953125" customWidth="1"/>
+    <col min="3" max="3" width="23.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -488,9 +544,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
@@ -499,9 +555,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
@@ -510,9 +566,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>3</v>
@@ -535,13 +591,13 @@
       <selection activeCell="A3" sqref="A3:XFD10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.26171875" customWidth="1"/>
+    <col min="1" max="1" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -549,19 +605,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
     </row>
@@ -578,13 +634,13 @@
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.26171875" customWidth="1"/>
+    <col min="1" max="1" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -592,19 +648,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
     </row>
@@ -617,27 +673,101 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2362296-9E5A-4FF5-B377-523F7E4FFCF2}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A89F3651-1282-425B-8D04-CB962D62DA53}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.7890625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60.54296875" customWidth="1"/>
+    <col min="3" max="3" width="28.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
+        <v>14</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="174" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="174" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="174" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding tag changes in runner file
</commit_message>
<xml_diff>
--- a/Ds-Algo/src/test/resources/TestData/registerUserName.xlsx
+++ b/Ds-Algo/src/test/resources/TestData/registerUserName.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sushm\eclipse-workspace\Ds-Algo-Git\ABS-Challengers\Ds-Algo\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98255B6C-C4DD-48B4-A615-88F2AC9A38A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0046FAED-579C-4B54-9DD2-56973569F7A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1800" yWindow="1800" windowWidth="17280" windowHeight="8994" xr2:uid="{D61A649E-4D94-4624-B804-336D99FF8C04}"/>
   </bookViews>
@@ -20,7 +20,6 @@
     <sheet name="practiceQuestions" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -130,7 +129,7 @@
   </si>
   <si>
     <r>
-      <t>ds_algo_abs_ch_60</t>
+      <t>ds_algo_abs_ch_70</t>
     </r>
     <r>
       <rPr>
@@ -143,10 +142,10 @@
     </r>
   </si>
   <si>
-    <t>ds_algo_abs_ch_601</t>
-  </si>
-  <si>
-    <t>ds_algo_abs_ch_602</t>
+    <t>ds_algo_abs_ch_701</t>
+  </si>
+  <si>
+    <t>ds_algo_abs_ch_702</t>
   </si>
 </sst>
 </file>

</xml_diff>